<commit_message>
added Few Test Cases In Add/View Village Test
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/Add_View_Village_Details.xlsx
+++ b/TestData/Excel_Files/Add_View_Village_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Hydologic_Core\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0335CF20-614E-4958-B835-A1816B258307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780B13C7-AB0F-4FCB-9C43-8505D1AC4678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E80F2CC9-4067-4EB4-8038-4F09443275B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Test Case id</t>
   </si>
@@ -81,19 +81,34 @@
   </si>
   <si>
     <t>Bhatkhedi</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>SU-T74</t>
+  </si>
+  <si>
+    <t>village_details.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F7F5F"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,8 +131,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF63B28D-ECF6-4756-9470-4782362BA7EC}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -467,9 +483,10 @@
     <col min="5" max="5" width="16.7265625" customWidth="1"/>
     <col min="6" max="6" width="22.81640625" customWidth="1"/>
     <col min="7" max="7" width="21.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,8 +508,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -515,7 +535,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -536,6 +556,14 @@
       </c>
       <c r="G3">
         <v>1234567890</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed functional test cases for add_view_village_details_test
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/Add_View_Village_Details.xlsx
+++ b/TestData/Excel_Files/Add_View_Village_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Hydologic_Core\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780B13C7-AB0F-4FCB-9C43-8505D1AC4678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2327007-33E3-4198-951A-80F8D49BA1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E80F2CC9-4067-4EB4-8038-4F09443275B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Test Case id</t>
   </si>
@@ -90,6 +90,30 @@
   </si>
   <si>
     <t>village_details.pdf</t>
+  </si>
+  <si>
+    <t>SU-T76</t>
+  </si>
+  <si>
+    <t>village_details.xlsx</t>
+  </si>
+  <si>
+    <t>SU-T77</t>
+  </si>
+  <si>
+    <t>Maksi</t>
+  </si>
+  <si>
+    <t>Ktahit</t>
+  </si>
+  <si>
+    <t>village_details (1).xlsx.crdownload</t>
+  </si>
+  <si>
+    <t>SU-T81</t>
+  </si>
+  <si>
+    <t>SU-T1084</t>
   </si>
 </sst>
 </file>
@@ -468,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF63B28D-ECF6-4756-9470-4782362BA7EC}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,7 +507,8 @@
     <col min="5" max="5" width="16.7265625" customWidth="1"/>
     <col min="6" max="6" width="22.81640625" customWidth="1"/>
     <col min="7" max="7" width="21.90625" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" customWidth="1"/>
+    <col min="8" max="8" width="29.6328125" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -566,6 +591,56 @@
         <v>17</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>